<commit_message>
* Now using OpenSSL's PRNG to generate AES key in Misc test * Better random anylisis. Xoroshiro is a good time vs uniformity deal compared to OpenSSL's PRNG, C's rand() and MT19937.
</commit_message>
<xml_diff>
--- a/RandomDistribution.xlsx
+++ b/RandomDistribution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nicolas\Documents\MGPCL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nicolas\Documents\mgpcl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>PRNG:</t>
   </si>
@@ -27,31 +27,55 @@
     <t>Xoroshiro</t>
   </si>
   <si>
+    <t>OpenSSL</t>
+  </si>
+  <si>
     <t>rand()</t>
   </si>
   <si>
-    <t>SUM</t>
+    <t>TOTAL</t>
   </si>
   <si>
-    <t>div</t>
+    <t>Max delta</t>
   </si>
   <si>
-    <t>EXPECTED</t>
+    <t>MT19937</t>
   </si>
   <si>
-    <t>Delta</t>
+    <t>Avg delta</t>
   </si>
   <si>
-    <t>Delta max</t>
+    <t>Computing time</t>
   </si>
   <si>
-    <t>Delta min</t>
+    <t>CPU: AMD FX-6100 overclocked @ 4.0 Ghz</t>
+  </si>
+  <si>
+    <t>OpenSSL 1.0.2f</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Best distribution, but quite slow</t>
+  </si>
+  <si>
+    <t>Fast and quite good distribution</t>
+  </si>
+  <si>
+    <t>Very slow, bad distribution, but secure for crypto</t>
+  </si>
+  <si>
+    <t>Fast, but bad distribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0\ \m\s"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -484,6 +508,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -529,8 +579,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -603,7 +666,76 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>p((n - 1)/20</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> &lt;= </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>X &lt; n/20</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -633,64 +765,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.0001999999999998E-2</c:v>
+                  <c:v>4.9747E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9922000000000001E-2</c:v>
+                  <c:v>4.9914E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9745999999999999E-2</c:v>
+                  <c:v>5.0185E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9449E-2</c:v>
+                  <c:v>4.9716999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0032E-2</c:v>
+                  <c:v>4.9743999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9856999999999999E-2</c:v>
+                  <c:v>4.9930000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0167000000000003E-2</c:v>
+                  <c:v>4.9979000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0032E-2</c:v>
+                  <c:v>4.9571999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0064999999999998E-2</c:v>
+                  <c:v>4.9981999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9854999999999997E-2</c:v>
+                  <c:v>5.0374000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9765999999999998E-2</c:v>
+                  <c:v>5.0292999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.9946999999999998E-2</c:v>
+                  <c:v>5.0123000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.9821999999999998E-2</c:v>
+                  <c:v>4.9605000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.0312999999999997E-2</c:v>
+                  <c:v>4.9799000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0464000000000002E-2</c:v>
+                  <c:v>5.0166000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0083999999999997E-2</c:v>
+                  <c:v>5.0223999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.9937000000000002E-2</c:v>
+                  <c:v>4.9845E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.0275E-2</c:v>
+                  <c:v>5.0250000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.0259999999999999E-2</c:v>
+                  <c:v>5.0130000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.0005000000000001E-2</c:v>
+                  <c:v>5.0421000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -700,7 +832,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>rand()</c:v>
+            <c:v>OpenSSL</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -719,70 +851,243 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.0014000000000003E-2</c:v>
+                  <c:v>4.9827999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9806999999999997E-2</c:v>
+                  <c:v>5.0381000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0153000000000003E-2</c:v>
+                  <c:v>4.9972999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.999E-2</c:v>
+                  <c:v>4.9743000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9993999999999997E-2</c:v>
+                  <c:v>5.0556999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9780999999999999E-2</c:v>
+                  <c:v>4.9554000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9688000000000003E-2</c:v>
+                  <c:v>4.9811000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>4.9797000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0226E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9709000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0220000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0067E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0172000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.972E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0152000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.9775E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>5.0104000000000003E-2</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9884999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0383999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.9942E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>rand()</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>random!$C$44:$C$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.9657E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0317000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0559E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9598000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0094E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9687000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9861000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0352000000000001E-2</c:v>
+                </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0126999999999998E-2</c:v>
+                  <c:v>4.9452999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.0215999999999997E-2</c:v>
+                  <c:v>4.9868000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9761E-2</c:v>
+                  <c:v>4.9887000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0015999999999998E-2</c:v>
+                  <c:v>5.0104999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.9918999999999998E-2</c:v>
+                  <c:v>5.0105999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9873000000000001E-2</c:v>
+                  <c:v>4.9910999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0182999999999998E-2</c:v>
+                  <c:v>5.0043999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0222999999999997E-2</c:v>
+                  <c:v>4.9953999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.0265999999999998E-2</c:v>
+                  <c:v>5.0224999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.9897999999999998E-2</c:v>
+                  <c:v>4.9779999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.0215999999999997E-2</c:v>
+                  <c:v>5.0401000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.9771000000000003E-2</c:v>
+                  <c:v>5.0140999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MT19937</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>random!$C$65:$C$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5.0299000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9998000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0279999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9910000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0259999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9778000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9813999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9832000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0001999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9896000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9660999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9870999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0312000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9999000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.9972999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.9914E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0067E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9978000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0206000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.9950000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -792,11 +1097,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1734038144"/>
-        <c:axId val="-1734041408"/>
+        <c:axId val="-843959744"/>
+        <c:axId val="-843967360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1734038144"/>
+        <c:axId val="-843959744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +1143,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734041408"/>
+        <c:crossAx val="-843967360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -846,11 +1151,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1734041408"/>
+        <c:axId val="-843967360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5.050000000000001E-2"/>
-          <c:min val="4.9400000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -899,7 +1202,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734038144"/>
+        <c:crossAx val="-843959744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1527,16 +1830,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1821,573 +2124,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>50002</v>
+        <v>49747</v>
       </c>
       <c r="C2">
-        <f>B2/$I$3</f>
-        <v>5.0001999999999998E-2</v>
+        <f>B2/$G$4</f>
+        <v>4.9747E-2</v>
       </c>
       <c r="D2">
-        <f>C2-$J$3</f>
-        <v>1.9999999999950613E-6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f>ABS(1/20-C2)</f>
+        <v>2.5300000000000322E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49922</v>
+        <v>49914</v>
       </c>
       <c r="C3">
-        <f>B3/$I$3</f>
-        <v>4.9922000000000001E-2</v>
+        <f t="shared" ref="C3:C66" si="0">B3/$G$4</f>
+        <v>4.9914E-2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">C3-$J$3</f>
-        <v>-7.8000000000001679E-5</v>
-      </c>
-      <c r="I3">
-        <f>SUM(B2:B21)</f>
-        <v>1000000</v>
-      </c>
-      <c r="J3">
-        <f>1/COUNT(A2:A21)</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D3:D66" si="1">ABS(1/20-C3)</f>
+        <v>8.6000000000002741E-5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>49746</v>
+        <v>50185</v>
       </c>
       <c r="C4">
-        <f>B4/$I$3</f>
-        <v>4.9745999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0185E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>-2.5400000000000422E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.8499999999999767E-4</v>
+      </c>
+      <c r="G4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>49449</v>
+        <v>49717</v>
       </c>
       <c r="C5">
-        <f>B5/$I$3</f>
-        <v>4.9449E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9716999999999997E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-5.5100000000000288E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.8300000000000547E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>50032</v>
+        <v>49744</v>
       </c>
       <c r="C6">
-        <f>B6/$I$3</f>
-        <v>5.0032E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9743999999999997E-2</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>3.1999999999997308E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.5600000000000622E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>49857</v>
+        <v>49930</v>
       </c>
       <c r="C7">
-        <f>B7/$I$3</f>
-        <v>4.9856999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9930000000000002E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-1.4300000000000423E-4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <f>MAX(D2:D21)</f>
-        <v>4.6399999999999914E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000617E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>50167</v>
+        <v>49979</v>
       </c>
       <c r="C8">
-        <f>B8/$I$3</f>
-        <v>5.0167000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9979000000000003E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.6700000000000048E-4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <f>-MIN(D2:D21)</f>
-        <v>5.5100000000000288E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.1000000000000185E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>50032</v>
+        <v>49572</v>
       </c>
       <c r="C9">
-        <f>B9/$I$3</f>
-        <v>5.0032E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9571999999999998E-2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>3.1999999999997308E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.2800000000000477E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>50065</v>
+        <v>49982</v>
       </c>
       <c r="C10">
-        <f>B10/$I$3</f>
-        <v>5.0064999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9981999999999999E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>6.4999999999995617E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.8000000000004124E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>49855</v>
+        <v>50374</v>
       </c>
       <c r="C11">
-        <f>B11/$I$3</f>
-        <v>4.9854999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0374000000000002E-2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-1.4500000000000624E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.7399999999999933E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>49766</v>
+        <v>50293</v>
       </c>
       <c r="C12">
-        <f>B12/$I$3</f>
-        <v>4.9765999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0292999999999997E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>-2.3400000000000504E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.9299999999999465E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>49947</v>
+        <v>50123</v>
       </c>
       <c r="C13">
-        <f>B13/$I$3</f>
-        <v>4.9946999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0123000000000001E-2</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>-5.3000000000004432E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.2299999999999811E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>49822</v>
+        <v>49605</v>
       </c>
       <c r="C14">
-        <f>B14/$I$3</f>
-        <v>4.9821999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9605000000000003E-2</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-1.7800000000000454E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.9499999999999952E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>50313</v>
+        <v>49799</v>
       </c>
       <c r="C15">
-        <f>B15/$I$3</f>
-        <v>5.0312999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9799000000000003E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>3.1299999999999384E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.0099999999999979E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>50464</v>
+        <v>50166</v>
       </c>
       <c r="C16">
-        <f>B16/$I$3</f>
-        <v>5.0464000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0166000000000002E-2</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>4.6399999999999914E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.6599999999999948E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>50084</v>
+        <v>50224</v>
       </c>
       <c r="C17">
-        <f>B17/$I$3</f>
-        <v>5.0083999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0223999999999998E-2</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>8.3999999999993802E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.2399999999999504E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>49937</v>
+        <v>49845</v>
       </c>
       <c r="C18">
-        <f>B18/$I$3</f>
-        <v>4.9937000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9845E-2</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>-6.3000000000000556E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.5500000000000236E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>50275</v>
+        <v>50250</v>
       </c>
       <c r="C19">
-        <f>B19/$I$3</f>
-        <v>5.0275E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0250000000000003E-2</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>2.7499999999999747E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000022E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>50260</v>
+        <v>50130</v>
       </c>
       <c r="C20">
-        <f>B20/$I$3</f>
-        <v>5.0259999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0130000000000001E-2</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>2.5999999999999635E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999817E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>50005</v>
+        <v>50421</v>
       </c>
       <c r="C21">
-        <f>B21/$I$3</f>
-        <v>5.0005000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0421000000000001E-2</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>4.9999999999980616E-6</v>
-      </c>
-      <c r="I21" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.2099999999999776E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="I22">
-        <f>SUM(B23:B42)</f>
-        <v>1000000</v>
-      </c>
-      <c r="J22">
-        <f>1/COUNT(A23:A42)</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="6"/>
+      <c r="H22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
       <c r="B23">
-        <v>50014</v>
+        <v>49828</v>
       </c>
       <c r="C23">
-        <f>B23/$I$22</f>
-        <v>5.0014000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9827999999999997E-2</v>
       </c>
       <c r="D23">
-        <f>C23-$J$22</f>
-        <v>1.4000000000000123E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.7200000000000548E-4</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <f>MAX($D$2:$D$21)</f>
+        <v>4.2800000000000477E-4</v>
+      </c>
+      <c r="I23" s="2">
+        <f>AVERAGE($D$2:$D$21)</f>
+        <v>2.1660000000000047E-4</v>
+      </c>
+      <c r="J23" s="3">
+        <v>82</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
-        <v>49807</v>
+        <v>50381</v>
       </c>
       <c r="C24">
-        <f>B24/$I$22</f>
-        <v>4.9806999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0381000000000002E-2</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D42" si="1">C24-$J$22</f>
-        <v>-1.9300000000000567E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.8099999999999939E-4</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <f>MAX($D$23:$D$42)</f>
+        <v>5.56999999999995E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f>AVERAGE($D$23:$D$42)</f>
+        <v>2.2630000000000046E-4</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1607</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25">
-        <v>50153</v>
+        <v>49973</v>
       </c>
       <c r="C25">
-        <f>B25/$I$22</f>
-        <v>5.0153000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9972999999999997E-2</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>1.5300000000000036E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.7000000000006186E-5</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="2">
+        <f>MAX($D$44:$D$63)</f>
+        <v>5.58999999999997E-4</v>
+      </c>
+      <c r="I25" s="2">
+        <f>AVERAGE($D$44:$D$63)</f>
+        <v>2.3439999999999954E-4</v>
+      </c>
+      <c r="J25" s="3">
+        <v>93</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26">
-        <v>49990</v>
+        <v>49743</v>
       </c>
       <c r="C26">
-        <f>B26/$I$22</f>
-        <v>4.999E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9743000000000002E-2</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>-1.0000000000003062E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.5700000000000028E-4</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="2">
+        <f>MAX($D$65:$D$84)</f>
+        <v>3.3900000000000596E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <f>AVERAGE($D$65:$D$84)</f>
+        <v>1.426000000000007E-4</v>
+      </c>
+      <c r="J26" s="3">
+        <v>383</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27">
-        <v>49994</v>
+        <v>50557</v>
       </c>
       <c r="C27">
-        <f>B27/$I$22</f>
-        <v>4.9993999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0556999999999998E-2</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>-6.0000000000060005E-6</v>
-      </c>
-      <c r="I27" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27">
-        <f>MAX(D23:D42)</f>
-        <v>2.6599999999999541E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.56999999999995E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>49781</v>
+        <v>49554</v>
       </c>
       <c r="C28">
-        <f>B28/$I$22</f>
-        <v>4.9780999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9554000000000001E-2</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>-2.1900000000000391E-4</v>
-      </c>
-      <c r="I28" t="s">
-        <v>8</v>
-      </c>
-      <c r="J28">
-        <f>-MIN(D23:D42)</f>
-        <v>3.1199999999999978E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.4600000000000195E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
       <c r="B29">
-        <v>49688</v>
+        <v>49811</v>
       </c>
       <c r="C29">
-        <f>B29/$I$22</f>
-        <v>4.9688000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9811000000000001E-2</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>-3.1199999999999978E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.8900000000000167E-4</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
       <c r="B30">
-        <v>50104</v>
+        <v>49797</v>
       </c>
       <c r="C30">
-        <f>B30/$I$22</f>
-        <v>5.0104000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9797000000000001E-2</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
-        <v>1.0399999999999993E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0300000000000179E-4</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
       <c r="B31">
-        <v>50127</v>
+        <v>50226</v>
       </c>
       <c r="C31">
-        <f>B31/$I$22</f>
-        <v>5.0126999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0226E-2</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>1.2699999999999517E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.2599999999999704E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
       <c r="B32">
-        <v>50216</v>
+        <v>49709</v>
       </c>
       <c r="C32">
-        <f>B32/$I$22</f>
-        <v>5.0215999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9709000000000003E-2</v>
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
-        <v>2.1599999999999397E-4</v>
+        <v>2.9099999999999959E-4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2395,15 +2739,15 @@
         <v>10</v>
       </c>
       <c r="B33">
-        <v>49761</v>
+        <v>50220</v>
       </c>
       <c r="C33">
-        <f>B33/$I$22</f>
-        <v>4.9761E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0220000000000001E-2</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>-2.390000000000031E-4</v>
+        <v>2.1999999999999797E-4</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2411,15 +2755,15 @@
         <v>11</v>
       </c>
       <c r="B34">
-        <v>50016</v>
+        <v>50067</v>
       </c>
       <c r="C34">
-        <f>B34/$I$22</f>
-        <v>5.0015999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0067E-2</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
-        <v>1.5999999999995185E-5</v>
+        <v>6.6999999999997617E-5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2427,15 +2771,15 @@
         <v>12</v>
       </c>
       <c r="B35">
-        <v>49919</v>
+        <v>50172</v>
       </c>
       <c r="C35">
-        <f>B35/$I$22</f>
-        <v>4.9918999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0172000000000001E-2</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
-        <v>-8.1000000000004679E-5</v>
+        <v>1.7199999999999854E-4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,15 +2787,15 @@
         <v>13</v>
       </c>
       <c r="B36">
-        <v>49873</v>
+        <v>49720</v>
       </c>
       <c r="C36">
-        <f>B36/$I$22</f>
-        <v>4.9873000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.972E-2</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>-1.2700000000000211E-4</v>
+        <v>2.8000000000000247E-4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,15 +2803,15 @@
         <v>14</v>
       </c>
       <c r="B37">
-        <v>50183</v>
+        <v>50152</v>
       </c>
       <c r="C37">
-        <f>B37/$I$22</f>
-        <v>5.0182999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0152000000000002E-2</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>1.8299999999999567E-4</v>
+        <v>1.5199999999999936E-4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,15 +2819,15 @@
         <v>15</v>
       </c>
       <c r="B38">
-        <v>50223</v>
+        <v>49775</v>
       </c>
       <c r="C38">
-        <f>B38/$I$22</f>
-        <v>5.0222999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9775E-2</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>2.2299999999999404E-4</v>
+        <v>2.2500000000000298E-4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2491,15 +2835,15 @@
         <v>16</v>
       </c>
       <c r="B39">
-        <v>50266</v>
+        <v>50104</v>
       </c>
       <c r="C39">
-        <f>B39/$I$22</f>
-        <v>5.0265999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0104000000000003E-2</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>2.6599999999999541E-4</v>
+        <v>1.0399999999999993E-4</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,15 +2851,15 @@
         <v>17</v>
       </c>
       <c r="B40">
-        <v>49898</v>
+        <v>49885</v>
       </c>
       <c r="C40">
-        <f>B40/$I$22</f>
-        <v>4.9897999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9884999999999999E-2</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>-1.0200000000000486E-4</v>
+        <v>1.1500000000000399E-4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2523,15 +2867,15 @@
         <v>18</v>
       </c>
       <c r="B41">
-        <v>50216</v>
+        <v>50384</v>
       </c>
       <c r="C41">
-        <f>B41/$I$22</f>
-        <v>5.0215999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0383999999999998E-2</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>2.1599999999999397E-4</v>
+        <v>3.8399999999999546E-4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2539,19 +2883,716 @@
         <v>19</v>
       </c>
       <c r="B42">
-        <v>49771</v>
+        <v>49942</v>
       </c>
       <c r="C42">
-        <f>B42/$I$22</f>
-        <v>4.9771000000000003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9942E-2</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
-        <v>-2.2900000000000004E-4</v>
+        <v>5.8000000000002494E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>49657</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>4.9657E-2</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>3.4300000000000302E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>50317</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>5.0317000000000001E-2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>3.1699999999999784E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>50559</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>5.0559E-2</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>5.58999999999997E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>49598</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>4.9598000000000003E-2</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>4.0199999999999958E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>50094</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>5.0094E-2</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>9.3999999999996864E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>49687</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>4.9687000000000002E-2</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>3.1300000000000078E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>49861</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>4.9861000000000003E-2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>1.3900000000000023E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>50352</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>5.0352000000000001E-2</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>3.5199999999999815E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>49453</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>4.9452999999999997E-2</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>5.4700000000000581E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>49868</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>4.9868000000000003E-2</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>1.3200000000000017E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>49887</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>4.9887000000000001E-2</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>1.1300000000000199E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>50105</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>5.0104999999999997E-2</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>1.0499999999999399E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>50106</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>5.0105999999999998E-2</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>1.0599999999999499E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>49911</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>4.9910999999999997E-2</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>8.9000000000005741E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>50044</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>5.0043999999999998E-2</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>4.3999999999995432E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59">
+        <v>49954</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>4.9953999999999998E-2</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>4.6000000000004371E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>50225</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>5.0224999999999999E-2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>2.2499999999999604E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>49780</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>4.9779999999999998E-2</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000491E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>18</v>
+      </c>
+      <c r="B62">
+        <v>50401</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>5.0401000000000001E-2</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>4.0099999999999858E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>19</v>
+      </c>
+      <c r="B63">
+        <v>50141</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>5.0140999999999998E-2</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>1.409999999999953E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>50299</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>5.0299000000000003E-2</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>2.9900000000000065E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>49998</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>4.9998000000000001E-2</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>2.0000000000020002E-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>50280</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C84" si="2">B67/$G$4</f>
+        <v>5.0279999999999998E-2</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D84" si="3">ABS(1/20-C67)</f>
+        <v>2.7999999999999553E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>49910</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="2"/>
+        <v>4.9910000000000003E-2</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>8.9999999999999802E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>50260</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="2"/>
+        <v>5.0259999999999999E-2</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>2.5999999999999635E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>49778</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>4.9778000000000003E-2</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="3"/>
+        <v>2.2199999999999998E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>49814</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="2"/>
+        <v>4.9813999999999997E-2</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>1.8600000000000561E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>49832</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="2"/>
+        <v>4.9832000000000001E-2</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="3"/>
+        <v>1.6800000000000148E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>8</v>
+      </c>
+      <c r="B73">
+        <v>50002</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="2"/>
+        <v>5.0001999999999998E-2</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>1.9999999999950613E-6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>9</v>
+      </c>
+      <c r="B74">
+        <v>49896</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>4.9896000000000003E-2</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="3"/>
+        <v>1.0399999999999993E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>49661</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>4.9660999999999997E-2</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="3"/>
+        <v>3.3900000000000596E-4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>49871</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>4.9870999999999999E-2</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="3"/>
+        <v>1.2900000000000411E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>12</v>
+      </c>
+      <c r="B77">
+        <v>50312</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>5.0312000000000003E-2</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="3"/>
+        <v>3.1199999999999978E-4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>13</v>
+      </c>
+      <c r="B78">
+        <v>49999</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="2"/>
+        <v>4.9999000000000002E-2</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="3"/>
+        <v>1.0000000000010001E-6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>49973</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="2"/>
+        <v>4.9972999999999997E-2</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="3"/>
+        <v>2.7000000000006186E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <v>49914</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="2"/>
+        <v>4.9914E-2</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="3"/>
+        <v>8.6000000000002741E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>16</v>
+      </c>
+      <c r="B81">
+        <v>50067</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="2"/>
+        <v>5.0067E-2</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="3"/>
+        <v>6.6999999999997617E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>17</v>
+      </c>
+      <c r="B82">
+        <v>49978</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="2"/>
+        <v>4.9978000000000002E-2</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="3"/>
+        <v>2.2000000000001185E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>18</v>
+      </c>
+      <c r="B83">
+        <v>50206</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="2"/>
+        <v>5.0206000000000001E-2</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="3"/>
+        <v>2.0599999999999785E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>19</v>
+      </c>
+      <c r="B84">
+        <v>49950</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="2"/>
+        <v>4.9950000000000001E-2</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="3"/>
+        <v>5.0000000000001432E-5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H23:H26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:I26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23:J26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>